<commit_message>
solved majority element i question
</commit_message>
<xml_diff>
--- a/Ultimate Leetcode DSA Sheet.xlsx
+++ b/Ultimate Leetcode DSA Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SDE\03. Java-DSA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\.SDE\04. Java-DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921D723B-93A2-4F82-AFC1-88227BB7AA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F860D4-05F6-422F-9D32-EC17B18468FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B38EDBA5-01EF-4A3D-9C7E-11FF357A630F}"/>
+    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11111" xr2:uid="{B38EDBA5-01EF-4A3D-9C7E-11FF357A630F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2450,18 +2450,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2505,9 +2493,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2516,6 +2501,21 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2835,23 +2835,23 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:L497"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A263" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A254" workbookViewId="0">
       <selection activeCell="B267" sqref="B267:H267"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
-    <col min="3" max="3" width="13.08984375" customWidth="1"/>
-    <col min="4" max="4" width="62.1796875" customWidth="1"/>
-    <col min="5" max="5" width="52.26953125" customWidth="1"/>
-    <col min="6" max="6" width="16.08984375" customWidth="1"/>
-    <col min="7" max="7" width="9.08984375" customWidth="1"/>
-    <col min="8" max="8" width="37.36328125" customWidth="1"/>
-    <col min="9" max="12" width="35.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.296875" customWidth="1"/>
+    <col min="3" max="3" width="13.09765625" customWidth="1"/>
+    <col min="4" max="4" width="62.19921875" customWidth="1"/>
+    <col min="5" max="5" width="52.296875" customWidth="1"/>
+    <col min="6" max="6" width="16.09765625" customWidth="1"/>
+    <col min="7" max="7" width="9.09765625" customWidth="1"/>
+    <col min="8" max="8" width="37.3984375" customWidth="1"/>
+    <col min="9" max="12" width="35.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="16"/>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
@@ -2859,18 +2859,18 @@
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
     </row>
-    <row r="3" spans="2:12" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="62" t="s">
+    <row r="3" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="80" t="s">
         <v>259</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>64</v>
       </c>
@@ -2893,18 +2893,18 @@
         <v>490</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="63" t="s">
+    <row r="5" spans="2:12" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="81" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>1</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>2</v>
       </c>
@@ -2958,7 +2958,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>3</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <v>4</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>5</v>
       </c>
@@ -3036,7 +3036,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <v>6</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <v>7</v>
       </c>
@@ -3088,7 +3088,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <v>8</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <v>9</v>
       </c>
@@ -3140,7 +3140,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <v>10</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <v>11</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <v>12</v>
       </c>
@@ -3218,7 +3218,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <v>13</v>
       </c>
@@ -3244,7 +3244,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <v>14</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <v>15</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <v>16</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <v>17</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <v>18</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <v>19</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <v>20</v>
       </c>
@@ -3426,7 +3426,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <v>21</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <v>22</v>
       </c>
@@ -3478,7 +3478,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <v>23</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29" s="3">
         <v>24</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <v>25</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" s="3">
         <v>26</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B32" s="3">
         <v>27</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B33" s="3">
         <v>28</v>
       </c>
@@ -3634,7 +3634,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B34" s="3">
         <v>29</v>
       </c>
@@ -3660,7 +3660,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B35" s="3">
         <v>30</v>
       </c>
@@ -3686,7 +3686,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B36" s="3">
         <v>31</v>
       </c>
@@ -3712,7 +3712,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B37" s="3">
         <v>32</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B38" s="3">
         <v>33</v>
       </c>
@@ -3764,7 +3764,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B39" s="3">
         <v>34</v>
       </c>
@@ -3790,7 +3790,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B40" s="3">
         <v>35</v>
       </c>
@@ -3816,7 +3816,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B41" s="3">
         <v>36</v>
       </c>
@@ -3842,7 +3842,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B42" s="3">
         <v>37</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B43" s="3">
         <v>38</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B44" s="3">
         <v>39</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B45" s="3">
         <v>40</v>
       </c>
@@ -3946,7 +3946,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B46" s="3">
         <v>41</v>
       </c>
@@ -3972,7 +3972,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B47" s="3">
         <v>42</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B48" s="3">
         <v>43</v>
       </c>
@@ -4024,7 +4024,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B49" s="3">
         <v>44</v>
       </c>
@@ -4050,7 +4050,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B50" s="3">
         <v>45</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B51" s="3">
         <v>46</v>
       </c>
@@ -4102,7 +4102,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B52" s="3">
         <v>47</v>
       </c>
@@ -4128,7 +4128,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B53" s="3">
         <v>48</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B54" s="3">
         <v>49</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B55" s="3">
         <v>50</v>
       </c>
@@ -4206,7 +4206,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B56" s="3">
         <v>51</v>
       </c>
@@ -4232,7 +4232,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B57" s="3">
         <v>52</v>
       </c>
@@ -4258,7 +4258,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B58" s="3">
         <v>53</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B59" s="3">
         <v>54</v>
       </c>
@@ -4310,7 +4310,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B60" s="3">
         <v>55</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B61" s="3">
         <v>56</v>
       </c>
@@ -4362,23 +4362,23 @@
         <v>317</v>
       </c>
     </row>
-    <row r="62" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="63" t="s">
+    <row r="62" spans="2:12" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="81" t="s">
         <v>67</v>
       </c>
-      <c r="C62" s="63"/>
-      <c r="D62" s="63"/>
-      <c r="E62" s="63"/>
-      <c r="F62" s="63"/>
-      <c r="G62" s="63"/>
-      <c r="H62" s="63"/>
+      <c r="C62" s="81"/>
+      <c r="D62" s="81"/>
+      <c r="E62" s="81"/>
+      <c r="F62" s="81"/>
+      <c r="G62" s="81"/>
+      <c r="H62" s="81"/>
       <c r="I62" s="43"/>
       <c r="J62" s="43"/>
       <c r="L62" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B63" s="9">
         <v>57</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B64" s="9">
         <v>58</v>
       </c>
@@ -4430,7 +4430,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B65" s="9">
         <v>59</v>
       </c>
@@ -4456,7 +4456,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B66" s="9">
         <v>60</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B67" s="9">
         <v>61</v>
       </c>
@@ -4508,7 +4508,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B68" s="9">
         <v>62</v>
       </c>
@@ -4534,7 +4534,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B69" s="9">
         <v>63</v>
       </c>
@@ -4560,7 +4560,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="70" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B70" s="9">
         <v>64</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B71" s="9">
         <v>65</v>
       </c>
@@ -4612,7 +4612,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B72" s="9">
         <v>66</v>
       </c>
@@ -4638,7 +4638,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B73" s="9">
         <v>67</v>
       </c>
@@ -4664,7 +4664,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B74" s="9">
         <v>68</v>
       </c>
@@ -4690,7 +4690,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B75" s="9">
         <v>69</v>
       </c>
@@ -4716,7 +4716,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B76" s="9">
         <v>70</v>
       </c>
@@ -4742,7 +4742,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B77" s="9">
         <v>71</v>
       </c>
@@ -4768,7 +4768,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B78" s="9">
         <v>72</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B79" s="9">
         <v>73</v>
       </c>
@@ -4820,7 +4820,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B80" s="9">
         <v>74</v>
       </c>
@@ -4846,23 +4846,23 @@
         <v>335</v>
       </c>
     </row>
-    <row r="81" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B81" s="63" t="s">
+    <row r="81" spans="2:12" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="C81" s="63"/>
-      <c r="D81" s="63"/>
-      <c r="E81" s="63"/>
-      <c r="F81" s="63"/>
-      <c r="G81" s="63"/>
-      <c r="H81" s="63"/>
+      <c r="C81" s="81"/>
+      <c r="D81" s="81"/>
+      <c r="E81" s="81"/>
+      <c r="F81" s="81"/>
+      <c r="G81" s="81"/>
+      <c r="H81" s="81"/>
       <c r="I81" s="43"/>
       <c r="J81" s="43"/>
       <c r="L81" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="82" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B82" s="3">
         <v>75</v>
       </c>
@@ -4888,7 +4888,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="83" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B83" s="3">
         <v>76</v>
       </c>
@@ -4914,7 +4914,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="84" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B84" s="3">
         <v>77</v>
       </c>
@@ -4940,7 +4940,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="85" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B85" s="3">
         <v>78</v>
       </c>
@@ -4966,7 +4966,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="86" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B86" s="3">
         <v>79</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="87" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B87" s="3">
         <v>80</v>
       </c>
@@ -5018,7 +5018,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="88" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B88" s="3">
         <v>81</v>
       </c>
@@ -5044,7 +5044,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="89" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B89" s="3">
         <v>82</v>
       </c>
@@ -5070,7 +5070,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="90" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B90" s="3">
         <v>83</v>
       </c>
@@ -5096,7 +5096,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="91" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B91" s="3">
         <v>84</v>
       </c>
@@ -5122,23 +5122,23 @@
         <v>345</v>
       </c>
     </row>
-    <row r="92" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B92" s="63" t="s">
+    <row r="92" spans="2:12" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B92" s="81" t="s">
         <v>117</v>
       </c>
-      <c r="C92" s="63"/>
-      <c r="D92" s="63"/>
-      <c r="E92" s="63"/>
-      <c r="F92" s="63"/>
-      <c r="G92" s="63"/>
-      <c r="H92" s="63"/>
+      <c r="C92" s="81"/>
+      <c r="D92" s="81"/>
+      <c r="E92" s="81"/>
+      <c r="F92" s="81"/>
+      <c r="G92" s="81"/>
+      <c r="H92" s="81"/>
       <c r="I92" s="43"/>
       <c r="J92" s="43"/>
       <c r="L92" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="93" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B93" s="14">
         <v>85</v>
       </c>
@@ -5166,7 +5166,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="94" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B94" s="14">
         <v>86</v>
       </c>
@@ -5192,7 +5192,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="95" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B95" s="14">
         <v>87</v>
       </c>
@@ -5218,7 +5218,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="96" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B96" s="14">
         <v>88</v>
       </c>
@@ -5244,7 +5244,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="97" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B97" s="14">
         <v>89</v>
       </c>
@@ -5270,7 +5270,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="98" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B98" s="14">
         <v>90</v>
       </c>
@@ -5296,7 +5296,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="99" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B99" s="14">
         <v>91</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="100" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B100" s="14">
         <v>92</v>
       </c>
@@ -5348,7 +5348,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="101" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B101" s="14">
         <v>93</v>
       </c>
@@ -5374,7 +5374,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="102" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B102" s="14">
         <v>94</v>
       </c>
@@ -5400,7 +5400,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="103" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B103" s="14">
         <v>95</v>
       </c>
@@ -5426,7 +5426,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="104" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B104" s="14">
         <v>96</v>
       </c>
@@ -5452,7 +5452,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="105" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B105" s="14">
         <v>97</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="106" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B106" s="14">
         <v>98</v>
       </c>
@@ -5504,7 +5504,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="107" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B107" s="14">
         <v>99</v>
       </c>
@@ -5530,7 +5530,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="108" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B108" s="14">
         <v>100</v>
       </c>
@@ -5556,7 +5556,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="109" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B109" s="14">
         <v>101</v>
       </c>
@@ -5582,7 +5582,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="110" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B110" s="14">
         <v>102</v>
       </c>
@@ -5608,7 +5608,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="111" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B111" s="14">
         <v>103</v>
       </c>
@@ -5634,7 +5634,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="112" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B112" s="14">
         <v>104</v>
       </c>
@@ -5660,7 +5660,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="113" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B113" s="14">
         <v>105</v>
       </c>
@@ -5686,7 +5686,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="114" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B114" s="14">
         <v>106</v>
       </c>
@@ -5712,7 +5712,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="115" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B115" s="14">
         <v>107</v>
       </c>
@@ -5738,7 +5738,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="116" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B116" s="14">
         <v>108</v>
       </c>
@@ -5764,7 +5764,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="117" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B117" s="14">
         <v>109</v>
       </c>
@@ -5790,7 +5790,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="118" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B118" s="14">
         <v>110</v>
       </c>
@@ -5816,7 +5816,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="119" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B119" s="14">
         <v>111</v>
       </c>
@@ -5842,7 +5842,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="120" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B120" s="14">
         <v>112</v>
       </c>
@@ -5868,7 +5868,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="121" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B121" s="14">
         <v>113</v>
       </c>
@@ -5894,7 +5894,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="122" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B122" s="14">
         <v>114</v>
       </c>
@@ -5920,7 +5920,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="123" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B123" s="14">
         <v>115</v>
       </c>
@@ -5946,7 +5946,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="124" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B124" s="14">
         <v>116</v>
       </c>
@@ -5972,7 +5972,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="125" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B125" s="14">
         <v>117</v>
       </c>
@@ -5998,7 +5998,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="126" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B126" s="14">
         <v>118</v>
       </c>
@@ -6024,7 +6024,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="127" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B127" s="14">
         <v>119</v>
       </c>
@@ -6050,7 +6050,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="128" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B128" s="14">
         <v>120</v>
       </c>
@@ -6076,7 +6076,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="129" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B129" s="14">
         <v>121</v>
       </c>
@@ -6102,7 +6102,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="130" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B130" s="14">
         <v>122</v>
       </c>
@@ -6128,7 +6128,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="131" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B131" s="14">
         <v>123</v>
       </c>
@@ -6154,7 +6154,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="132" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B132" s="14">
         <v>124</v>
       </c>
@@ -6180,7 +6180,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="133" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B133" s="14">
         <v>125</v>
       </c>
@@ -6206,7 +6206,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="134" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B134" s="14">
         <v>126</v>
       </c>
@@ -6232,7 +6232,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="135" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B135" s="14">
         <v>127</v>
       </c>
@@ -6258,7 +6258,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="136" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B136" s="14">
         <v>128</v>
       </c>
@@ -6284,7 +6284,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="137" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B137" s="14">
         <v>129</v>
       </c>
@@ -6310,7 +6310,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="138" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B138" s="14">
         <v>130</v>
       </c>
@@ -6336,7 +6336,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="139" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B139" s="14">
         <v>131</v>
       </c>
@@ -6362,7 +6362,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="140" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B140" s="14">
         <v>132</v>
       </c>
@@ -6388,7 +6388,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="141" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B141" s="14">
         <v>133</v>
       </c>
@@ -6414,7 +6414,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="142" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B142" s="14">
         <v>134</v>
       </c>
@@ -6440,7 +6440,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="143" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B143" s="14">
         <v>135</v>
       </c>
@@ -6466,7 +6466,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="144" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B144" s="14">
         <v>136</v>
       </c>
@@ -6492,7 +6492,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="145" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B145" s="14">
         <v>137</v>
       </c>
@@ -6518,7 +6518,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="146" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B146" s="14">
         <v>138</v>
       </c>
@@ -6544,7 +6544,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="147" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B147" s="14">
         <v>139</v>
       </c>
@@ -6570,7 +6570,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="148" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B148" s="14">
         <v>140</v>
       </c>
@@ -6596,7 +6596,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="149" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B149" s="14">
         <v>141</v>
       </c>
@@ -6622,7 +6622,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="150" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B150" s="14">
         <v>142</v>
       </c>
@@ -6648,7 +6648,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="151" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B151" s="14">
         <v>143</v>
       </c>
@@ -6674,7 +6674,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="152" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B152" s="14">
         <v>144</v>
       </c>
@@ -6700,7 +6700,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="153" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B153" s="14">
         <v>145</v>
       </c>
@@ -6726,7 +6726,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="154" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B154" s="14">
         <v>146</v>
       </c>
@@ -6752,7 +6752,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="155" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B155" s="14">
         <v>147</v>
       </c>
@@ -6778,7 +6778,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="156" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B156" s="14">
         <v>148</v>
       </c>
@@ -6804,7 +6804,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="157" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B157" s="14">
         <v>149</v>
       </c>
@@ -6830,7 +6830,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="158" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B158" s="14">
         <v>150</v>
       </c>
@@ -6856,7 +6856,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="159" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="159" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B159" s="14">
         <v>151</v>
       </c>
@@ -6882,7 +6882,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="160" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B160" s="14">
         <v>152</v>
       </c>
@@ -6908,7 +6908,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="161" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="161" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B161" s="14">
         <v>153</v>
       </c>
@@ -6934,7 +6934,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="162" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B162" s="14">
         <v>154</v>
       </c>
@@ -6960,7 +6960,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="163" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="163" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B163" s="14">
         <v>155</v>
       </c>
@@ -6986,7 +6986,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="164" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="164" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B164" s="14">
         <v>156</v>
       </c>
@@ -7012,7 +7012,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="165" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="165" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B165" s="14">
         <v>157</v>
       </c>
@@ -7038,7 +7038,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="166" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="166" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B166" s="14">
         <v>158</v>
       </c>
@@ -7064,7 +7064,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="167" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="167" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B167" s="14">
         <v>159</v>
       </c>
@@ -7090,7 +7090,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="168" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="168" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B168" s="14">
         <v>160</v>
       </c>
@@ -7116,7 +7116,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="169" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="169" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B169" s="14">
         <v>161</v>
       </c>
@@ -7142,7 +7142,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="170" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="170" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B170" s="14">
         <v>162</v>
       </c>
@@ -7168,7 +7168,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="171" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="171" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B171" s="14">
         <v>163</v>
       </c>
@@ -7194,7 +7194,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="172" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="172" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B172" s="14">
         <v>164</v>
       </c>
@@ -7220,7 +7220,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="173" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="173" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B173" s="14">
         <v>165</v>
       </c>
@@ -7246,7 +7246,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="174" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="174" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B174" s="14">
         <v>166</v>
       </c>
@@ -7272,7 +7272,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="175" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="175" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B175" s="14">
         <v>167</v>
       </c>
@@ -7298,7 +7298,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="176" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="176" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B176" s="14">
         <v>168</v>
       </c>
@@ -7324,7 +7324,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="177" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="177" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B177" s="14">
         <v>169</v>
       </c>
@@ -7350,7 +7350,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="178" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="178" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B178" s="14">
         <v>170</v>
       </c>
@@ -7376,7 +7376,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="179" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="179" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B179" s="14">
         <v>171</v>
       </c>
@@ -7402,7 +7402,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="180" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="180" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B180" s="14">
         <v>172</v>
       </c>
@@ -7428,7 +7428,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="181" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="181" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B181" s="14">
         <v>173</v>
       </c>
@@ -7454,7 +7454,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="182" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="182" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B182" s="14">
         <v>174</v>
       </c>
@@ -7480,7 +7480,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="183" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="183" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B183" s="14">
         <v>175</v>
       </c>
@@ -7506,7 +7506,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="184" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="184" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B184" s="14">
         <v>176</v>
       </c>
@@ -7532,7 +7532,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="185" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="185" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B185" s="14">
         <v>177</v>
       </c>
@@ -7558,7 +7558,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="186" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="186" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B186" s="14">
         <v>178</v>
       </c>
@@ -7584,7 +7584,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="187" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="187" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B187" s="14">
         <v>179</v>
       </c>
@@ -7610,7 +7610,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="188" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="188" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B188" s="14">
         <v>180</v>
       </c>
@@ -7636,7 +7636,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="189" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="189" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B189" s="14">
         <v>181</v>
       </c>
@@ -7662,7 +7662,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="190" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="190" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B190" s="14">
         <v>182</v>
       </c>
@@ -7688,7 +7688,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="191" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="191" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B191" s="14">
         <v>183</v>
       </c>
@@ -7714,7 +7714,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="192" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="192" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B192" s="14">
         <v>184</v>
       </c>
@@ -7740,7 +7740,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="193" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="193" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B193" s="14">
         <v>185</v>
       </c>
@@ -7766,7 +7766,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="194" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="194" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B194" s="14">
         <v>186</v>
       </c>
@@ -7792,7 +7792,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="195" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="195" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B195" s="14">
         <v>187</v>
       </c>
@@ -7818,7 +7818,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="196" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="196" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B196" s="14">
         <v>188</v>
       </c>
@@ -7844,7 +7844,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="197" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="197" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B197" s="14">
         <v>189</v>
       </c>
@@ -7870,7 +7870,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="198" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="198" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B198" s="14">
         <v>190</v>
       </c>
@@ -7896,7 +7896,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="199" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="199" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B199" s="14">
         <v>191</v>
       </c>
@@ -7922,7 +7922,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="200" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="200" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B200" s="14">
         <v>192</v>
       </c>
@@ -7948,7 +7948,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="201" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="201" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B201" s="14">
         <v>193</v>
       </c>
@@ -7974,7 +7974,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="202" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="202" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B202" s="14">
         <v>194</v>
       </c>
@@ -8000,7 +8000,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="203" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="203" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B203" s="14">
         <v>195</v>
       </c>
@@ -8026,7 +8026,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="204" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="204" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B204" s="14">
         <v>196</v>
       </c>
@@ -8052,7 +8052,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="205" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="205" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B205" s="14">
         <v>197</v>
       </c>
@@ -8078,7 +8078,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="206" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="206" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B206" s="14">
         <v>198</v>
       </c>
@@ -8104,7 +8104,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="207" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="207" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B207" s="14">
         <v>199</v>
       </c>
@@ -8130,7 +8130,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="208" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="208" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B208" s="14">
         <v>200</v>
       </c>
@@ -8156,7 +8156,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="209" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="209" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B209" s="14">
         <v>201</v>
       </c>
@@ -8182,7 +8182,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="210" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="210" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B210" s="14">
         <v>202</v>
       </c>
@@ -8208,7 +8208,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="211" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="211" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B211" s="14">
         <v>203</v>
       </c>
@@ -8234,7 +8234,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="212" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="212" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B212" s="14">
         <v>204</v>
       </c>
@@ -8260,7 +8260,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="213" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="213" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B213" s="14">
         <v>205</v>
       </c>
@@ -8286,7 +8286,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="214" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="214" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B214" s="14">
         <v>206</v>
       </c>
@@ -8312,7 +8312,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="215" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="215" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B215" s="14">
         <v>207</v>
       </c>
@@ -8338,7 +8338,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="216" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="216" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B216" s="14">
         <v>208</v>
       </c>
@@ -8364,7 +8364,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="217" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="217" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B217" s="14">
         <v>209</v>
       </c>
@@ -8390,23 +8390,23 @@
         <v>470</v>
       </c>
     </row>
-    <row r="218" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B218" s="63" t="s">
+    <row r="218" spans="2:12" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B218" s="81" t="s">
         <v>103</v>
       </c>
-      <c r="C218" s="63"/>
-      <c r="D218" s="63"/>
-      <c r="E218" s="63"/>
-      <c r="F218" s="63"/>
-      <c r="G218" s="63"/>
-      <c r="H218" s="63"/>
+      <c r="C218" s="81"/>
+      <c r="D218" s="81"/>
+      <c r="E218" s="81"/>
+      <c r="F218" s="81"/>
+      <c r="G218" s="81"/>
+      <c r="H218" s="81"/>
       <c r="I218" s="43"/>
       <c r="J218" s="43"/>
       <c r="L218" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="219" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="219" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B219" s="14">
         <v>210</v>
       </c>
@@ -8432,7 +8432,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="220" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="220" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B220" s="14">
         <v>211</v>
       </c>
@@ -8458,7 +8458,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="221" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="221" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B221" s="14">
         <v>212</v>
       </c>
@@ -8484,7 +8484,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="222" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="222" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B222" s="14">
         <v>213</v>
       </c>
@@ -8510,7 +8510,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="223" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="223" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B223" s="14">
         <v>214</v>
       </c>
@@ -8536,7 +8536,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="224" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="224" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B224" s="14">
         <v>215</v>
       </c>
@@ -8562,7 +8562,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="225" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="225" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B225" s="14">
         <v>216</v>
       </c>
@@ -8588,7 +8588,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="226" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="226" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B226" s="14">
         <v>217</v>
       </c>
@@ -8614,7 +8614,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="227" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="227" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B227" s="14">
         <v>218</v>
       </c>
@@ -8640,7 +8640,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="228" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B228" s="14">
         <v>219</v>
       </c>
@@ -8666,7 +8666,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="229" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="229" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B229" s="14">
         <v>220</v>
       </c>
@@ -8692,7 +8692,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="230" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="230" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B230" s="14">
         <v>221</v>
       </c>
@@ -8718,7 +8718,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="231" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="231" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B231" s="14">
         <v>222</v>
       </c>
@@ -8744,7 +8744,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="232" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="232" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B232" s="14">
         <v>223</v>
       </c>
@@ -8770,7 +8770,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="233" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="233" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B233" s="14">
         <v>224</v>
       </c>
@@ -8796,7 +8796,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="234" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="234" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B234" s="14">
         <v>225</v>
       </c>
@@ -8822,7 +8822,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="235" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="235" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B235" s="14">
         <v>226</v>
       </c>
@@ -8848,7 +8848,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="236" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="236" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B236" s="14">
         <v>227</v>
       </c>
@@ -8874,7 +8874,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="237" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="237" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B237" s="14">
         <v>228</v>
       </c>
@@ -8900,31 +8900,31 @@
         <v>489</v>
       </c>
     </row>
-    <row r="238" spans="2:12" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B238" s="60" t="s">
+    <row r="238" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B238" s="78" t="s">
         <v>679</v>
       </c>
-      <c r="C238" s="61"/>
-      <c r="D238" s="61"/>
-      <c r="E238" s="61"/>
-      <c r="F238" s="61"/>
-      <c r="G238" s="61"/>
-      <c r="H238" s="61"/>
-    </row>
-    <row r="239" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B239" s="75">
+      <c r="C238" s="79"/>
+      <c r="D238" s="79"/>
+      <c r="E238" s="79"/>
+      <c r="F238" s="79"/>
+      <c r="G238" s="79"/>
+      <c r="H238" s="79"/>
+    </row>
+    <row r="239" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B239" s="71">
         <v>229</v>
       </c>
-      <c r="C239" s="75">
+      <c r="C239" s="71">
         <v>1480</v>
       </c>
       <c r="D239" s="4" t="s">
         <v>618</v>
       </c>
-      <c r="E239" s="76" t="s">
+      <c r="E239" s="72" t="s">
         <v>646</v>
       </c>
-      <c r="F239" s="77" t="s">
+      <c r="F239" s="73" t="s">
         <v>5</v>
       </c>
       <c r="G239" s="8"/>
@@ -8933,20 +8933,20 @@
       </c>
       <c r="I239" s="43"/>
     </row>
-    <row r="240" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B240" s="75">
+    <row r="240" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B240" s="71">
         <v>230</v>
       </c>
-      <c r="C240" s="75">
+      <c r="C240" s="71">
         <v>2574</v>
       </c>
       <c r="D240" s="4" t="s">
         <v>619</v>
       </c>
-      <c r="E240" s="76" t="s">
+      <c r="E240" s="72" t="s">
         <v>646</v>
       </c>
-      <c r="F240" s="77" t="s">
+      <c r="F240" s="73" t="s">
         <v>5</v>
       </c>
       <c r="G240" s="8"/>
@@ -8955,20 +8955,20 @@
       </c>
       <c r="I240" s="43"/>
     </row>
-    <row r="241" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B241" s="75">
+    <row r="241" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B241" s="71">
         <v>231</v>
       </c>
-      <c r="C241" s="75">
+      <c r="C241" s="71">
         <v>2485</v>
       </c>
       <c r="D241" s="4" t="s">
         <v>620</v>
       </c>
-      <c r="E241" s="76" t="s">
+      <c r="E241" s="72" t="s">
         <v>647</v>
       </c>
-      <c r="F241" s="77" t="s">
+      <c r="F241" s="73" t="s">
         <v>5</v>
       </c>
       <c r="G241" s="8"/>
@@ -8977,20 +8977,20 @@
       </c>
       <c r="I241" s="43"/>
     </row>
-    <row r="242" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B242" s="75">
+    <row r="242" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B242" s="71">
         <v>232</v>
       </c>
-      <c r="C242" s="75">
+      <c r="C242" s="71">
         <v>1732</v>
       </c>
       <c r="D242" s="4" t="s">
         <v>621</v>
       </c>
-      <c r="E242" s="76" t="s">
+      <c r="E242" s="72" t="s">
         <v>646</v>
       </c>
-      <c r="F242" s="77" t="s">
+      <c r="F242" s="73" t="s">
         <v>5</v>
       </c>
       <c r="G242" s="8"/>
@@ -8999,20 +8999,20 @@
       </c>
       <c r="I242" s="43"/>
     </row>
-    <row r="243" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B243" s="75">
+    <row r="243" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B243" s="71">
         <v>233</v>
       </c>
-      <c r="C243" s="75">
+      <c r="C243" s="71">
         <v>1588</v>
       </c>
       <c r="D243" s="4" t="s">
         <v>622</v>
       </c>
-      <c r="E243" s="76" t="s">
+      <c r="E243" s="72" t="s">
         <v>648</v>
       </c>
-      <c r="F243" s="77" t="s">
+      <c r="F243" s="73" t="s">
         <v>5</v>
       </c>
       <c r="G243" s="8"/>
@@ -9021,20 +9021,20 @@
       </c>
       <c r="I243" s="43"/>
     </row>
-    <row r="244" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B244" s="75">
+    <row r="244" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B244" s="71">
         <v>234</v>
       </c>
-      <c r="C244" s="75">
+      <c r="C244" s="71">
         <v>3028</v>
       </c>
       <c r="D244" s="4" t="s">
         <v>623</v>
       </c>
-      <c r="E244" s="76" t="s">
+      <c r="E244" s="72" t="s">
         <v>649</v>
       </c>
-      <c r="F244" s="77" t="s">
+      <c r="F244" s="73" t="s">
         <v>5</v>
       </c>
       <c r="G244" s="8"/>
@@ -9043,20 +9043,20 @@
       </c>
       <c r="I244" s="43"/>
     </row>
-    <row r="245" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B245" s="75">
+    <row r="245" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B245" s="71">
         <v>235</v>
       </c>
-      <c r="C245" s="75">
+      <c r="C245" s="71">
         <v>1991</v>
       </c>
       <c r="D245" s="4" t="s">
         <v>624</v>
       </c>
-      <c r="E245" s="76" t="s">
+      <c r="E245" s="72" t="s">
         <v>646</v>
       </c>
-      <c r="F245" s="77" t="s">
+      <c r="F245" s="73" t="s">
         <v>5</v>
       </c>
       <c r="G245" s="8"/>
@@ -9065,20 +9065,20 @@
       </c>
       <c r="I245" s="43"/>
     </row>
-    <row r="246" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B246" s="75">
+    <row r="246" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B246" s="71">
         <v>236</v>
       </c>
-      <c r="C246" s="75">
+      <c r="C246" s="71">
         <v>1413</v>
       </c>
       <c r="D246" s="4" t="s">
         <v>625</v>
       </c>
-      <c r="E246" s="76" t="s">
+      <c r="E246" s="72" t="s">
         <v>646</v>
       </c>
-      <c r="F246" s="77" t="s">
+      <c r="F246" s="73" t="s">
         <v>5</v>
       </c>
       <c r="G246" s="8"/>
@@ -9087,20 +9087,20 @@
       </c>
       <c r="I246" s="43"/>
     </row>
-    <row r="247" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B247" s="75">
+    <row r="247" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B247" s="71">
         <v>237</v>
       </c>
-      <c r="C247" s="75">
+      <c r="C247" s="71">
         <v>724</v>
       </c>
       <c r="D247" s="4" t="s">
         <v>626</v>
       </c>
-      <c r="E247" s="76" t="s">
+      <c r="E247" s="72" t="s">
         <v>646</v>
       </c>
-      <c r="F247" s="77" t="s">
+      <c r="F247" s="73" t="s">
         <v>5</v>
       </c>
       <c r="G247" s="8"/>
@@ -9109,20 +9109,20 @@
       </c>
       <c r="I247" s="43"/>
     </row>
-    <row r="248" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B248" s="75">
+    <row r="248" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B248" s="71">
         <v>238</v>
       </c>
-      <c r="C248" s="75">
+      <c r="C248" s="71">
         <v>1829</v>
       </c>
       <c r="D248" s="4" t="s">
         <v>627</v>
       </c>
-      <c r="E248" s="76" t="s">
+      <c r="E248" s="72" t="s">
         <v>650</v>
       </c>
-      <c r="F248" s="78" t="s">
+      <c r="F248" s="74" t="s">
         <v>42</v>
       </c>
       <c r="G248" s="8"/>
@@ -9131,20 +9131,20 @@
       </c>
       <c r="I248" s="43"/>
     </row>
-    <row r="249" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B249" s="75">
+    <row r="249" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B249" s="71">
         <v>239</v>
       </c>
-      <c r="C249" s="75">
+      <c r="C249" s="71">
         <v>1310</v>
       </c>
       <c r="D249" s="4" t="s">
         <v>628</v>
       </c>
-      <c r="E249" s="76" t="s">
+      <c r="E249" s="72" t="s">
         <v>650</v>
       </c>
-      <c r="F249" s="78" t="s">
+      <c r="F249" s="74" t="s">
         <v>42</v>
       </c>
       <c r="G249" s="8"/>
@@ -9153,20 +9153,20 @@
       </c>
       <c r="I249" s="43"/>
     </row>
-    <row r="250" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B250" s="75">
+    <row r="250" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B250" s="71">
         <v>240</v>
       </c>
-      <c r="C250" s="75">
+      <c r="C250" s="71">
         <v>370</v>
       </c>
       <c r="D250" s="4" t="s">
         <v>629</v>
       </c>
-      <c r="E250" s="76" t="s">
+      <c r="E250" s="72" t="s">
         <v>646</v>
       </c>
-      <c r="F250" s="78" t="s">
+      <c r="F250" s="74" t="s">
         <v>42</v>
       </c>
       <c r="G250" s="8"/>
@@ -9175,20 +9175,20 @@
       </c>
       <c r="I250" s="43"/>
     </row>
-    <row r="251" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B251" s="75">
+    <row r="251" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B251" s="71">
         <v>241</v>
       </c>
-      <c r="C251" s="75">
+      <c r="C251" s="71">
         <v>2640</v>
       </c>
       <c r="D251" s="4" t="s">
         <v>630</v>
       </c>
-      <c r="E251" s="76" t="s">
+      <c r="E251" s="72" t="s">
         <v>646</v>
       </c>
-      <c r="F251" s="78" t="s">
+      <c r="F251" s="74" t="s">
         <v>42</v>
       </c>
       <c r="G251" s="8"/>
@@ -9197,20 +9197,20 @@
       </c>
       <c r="I251" s="43"/>
     </row>
-    <row r="252" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B252" s="75">
+    <row r="252" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B252" s="71">
         <v>242</v>
       </c>
-      <c r="C252" s="75">
+      <c r="C252" s="71">
         <v>1685</v>
       </c>
       <c r="D252" s="4" t="s">
         <v>631</v>
       </c>
-      <c r="E252" s="76" t="s">
+      <c r="E252" s="72" t="s">
         <v>648</v>
       </c>
-      <c r="F252" s="78" t="s">
+      <c r="F252" s="74" t="s">
         <v>42</v>
       </c>
       <c r="G252" s="8"/>
@@ -9219,20 +9219,20 @@
       </c>
       <c r="I252" s="43"/>
     </row>
-    <row r="253" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B253" s="75">
+    <row r="253" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B253" s="71">
         <v>243</v>
       </c>
-      <c r="C253" s="75">
+      <c r="C253" s="71">
         <v>238</v>
       </c>
       <c r="D253" s="4" t="s">
         <v>632</v>
       </c>
-      <c r="E253" s="76" t="s">
+      <c r="E253" s="72" t="s">
         <v>646</v>
       </c>
-      <c r="F253" s="78" t="s">
+      <c r="F253" s="74" t="s">
         <v>42</v>
       </c>
       <c r="G253" s="8"/>
@@ -9241,20 +9241,20 @@
       </c>
       <c r="I253" s="43"/>
     </row>
-    <row r="254" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B254" s="75">
+    <row r="254" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B254" s="71">
         <v>244</v>
       </c>
-      <c r="C254" s="75">
+      <c r="C254" s="71">
         <v>2237</v>
       </c>
       <c r="D254" s="4" t="s">
         <v>633</v>
       </c>
-      <c r="E254" s="76" t="s">
+      <c r="E254" s="72" t="s">
         <v>646</v>
       </c>
-      <c r="F254" s="78" t="s">
+      <c r="F254" s="74" t="s">
         <v>42</v>
       </c>
       <c r="G254" s="8"/>
@@ -9263,20 +9263,20 @@
       </c>
       <c r="I254" s="43"/>
     </row>
-    <row r="255" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B255" s="75">
+    <row r="255" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B255" s="71">
         <v>245</v>
       </c>
-      <c r="C255" s="75">
+      <c r="C255" s="71">
         <v>1664</v>
       </c>
       <c r="D255" s="4" t="s">
         <v>634</v>
       </c>
-      <c r="E255" s="76" t="s">
+      <c r="E255" s="72" t="s">
         <v>646</v>
       </c>
-      <c r="F255" s="78" t="s">
+      <c r="F255" s="74" t="s">
         <v>42</v>
       </c>
       <c r="G255" s="8"/>
@@ -9285,20 +9285,20 @@
       </c>
       <c r="I255" s="43"/>
     </row>
-    <row r="256" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B256" s="75">
+    <row r="256" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B256" s="71">
         <v>246</v>
       </c>
-      <c r="C256" s="75">
+      <c r="C256" s="71">
         <v>2219</v>
       </c>
       <c r="D256" s="4" t="s">
         <v>635</v>
       </c>
-      <c r="E256" s="76" t="s">
+      <c r="E256" s="72" t="s">
         <v>646</v>
       </c>
-      <c r="F256" s="78" t="s">
+      <c r="F256" s="74" t="s">
         <v>42</v>
       </c>
       <c r="G256" s="8"/>
@@ -9307,20 +9307,20 @@
       </c>
       <c r="I256" s="43"/>
     </row>
-    <row r="257" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B257" s="75">
+    <row r="257" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B257" s="71">
         <v>247</v>
       </c>
-      <c r="C257" s="75">
+      <c r="C257" s="71">
         <v>1109</v>
       </c>
       <c r="D257" s="4" t="s">
         <v>636</v>
       </c>
-      <c r="E257" s="76" t="s">
+      <c r="E257" s="72" t="s">
         <v>646</v>
       </c>
-      <c r="F257" s="78" t="s">
+      <c r="F257" s="74" t="s">
         <v>42</v>
       </c>
       <c r="G257" s="8"/>
@@ -9329,20 +9329,20 @@
       </c>
       <c r="I257" s="43"/>
     </row>
-    <row r="258" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B258" s="75">
+    <row r="258" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B258" s="71">
         <v>248</v>
       </c>
-      <c r="C258" s="75">
+      <c r="C258" s="71">
         <v>2270</v>
       </c>
       <c r="D258" s="4" t="s">
         <v>637</v>
       </c>
-      <c r="E258" s="76" t="s">
+      <c r="E258" s="72" t="s">
         <v>646</v>
       </c>
-      <c r="F258" s="78" t="s">
+      <c r="F258" s="74" t="s">
         <v>42</v>
       </c>
       <c r="G258" s="8"/>
@@ -9351,20 +9351,20 @@
       </c>
       <c r="I258" s="43"/>
     </row>
-    <row r="259" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B259" s="75">
+    <row r="259" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B259" s="71">
         <v>249</v>
       </c>
-      <c r="C259" s="75">
+      <c r="C259" s="71">
         <v>2256</v>
       </c>
       <c r="D259" s="4" t="s">
         <v>638</v>
       </c>
-      <c r="E259" s="76" t="s">
+      <c r="E259" s="72" t="s">
         <v>646</v>
       </c>
-      <c r="F259" s="78" t="s">
+      <c r="F259" s="74" t="s">
         <v>42</v>
       </c>
       <c r="G259" s="8"/>
@@ -9373,20 +9373,20 @@
       </c>
       <c r="I259" s="43"/>
     </row>
-    <row r="260" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B260" s="75">
+    <row r="260" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B260" s="71">
         <v>250</v>
       </c>
-      <c r="C260" s="75">
+      <c r="C260" s="71">
         <v>3096</v>
       </c>
       <c r="D260" s="4" t="s">
         <v>639</v>
       </c>
-      <c r="E260" s="76" t="s">
+      <c r="E260" s="72" t="s">
         <v>646</v>
       </c>
-      <c r="F260" s="78" t="s">
+      <c r="F260" s="74" t="s">
         <v>42</v>
       </c>
       <c r="G260" s="8"/>
@@ -9395,20 +9395,20 @@
       </c>
       <c r="I260" s="43"/>
     </row>
-    <row r="261" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B261" s="75">
+    <row r="261" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B261" s="71">
         <v>251</v>
       </c>
-      <c r="C261" s="75">
+      <c r="C261" s="71">
         <v>3147</v>
       </c>
       <c r="D261" s="4" t="s">
         <v>640</v>
       </c>
-      <c r="E261" s="76" t="s">
+      <c r="E261" s="72" t="s">
         <v>646</v>
       </c>
-      <c r="F261" s="78" t="s">
+      <c r="F261" s="74" t="s">
         <v>42</v>
       </c>
       <c r="G261" s="8"/>
@@ -9417,20 +9417,20 @@
       </c>
       <c r="I261" s="43"/>
     </row>
-    <row r="262" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B262" s="75">
+    <row r="262" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B262" s="71">
         <v>252</v>
       </c>
-      <c r="C262" s="75">
+      <c r="C262" s="71">
         <v>2438</v>
       </c>
       <c r="D262" s="4" t="s">
         <v>641</v>
       </c>
-      <c r="E262" s="76" t="s">
+      <c r="E262" s="72" t="s">
         <v>650</v>
       </c>
-      <c r="F262" s="78" t="s">
+      <c r="F262" s="74" t="s">
         <v>42</v>
       </c>
       <c r="G262" s="8"/>
@@ -9439,20 +9439,20 @@
       </c>
       <c r="I262" s="43"/>
     </row>
-    <row r="263" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B263" s="75">
+    <row r="263" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B263" s="71">
         <v>253</v>
       </c>
-      <c r="C263" s="75">
+      <c r="C263" s="71">
         <v>2145</v>
       </c>
       <c r="D263" s="4" t="s">
         <v>642</v>
       </c>
-      <c r="E263" s="76" t="s">
+      <c r="E263" s="72" t="s">
         <v>646</v>
       </c>
-      <c r="F263" s="78" t="s">
+      <c r="F263" s="74" t="s">
         <v>42</v>
       </c>
       <c r="G263" s="8"/>
@@ -9461,20 +9461,20 @@
       </c>
       <c r="I263" s="43"/>
     </row>
-    <row r="264" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B264" s="75">
+    <row r="264" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B264" s="71">
         <v>254</v>
       </c>
-      <c r="C264" s="75">
+      <c r="C264" s="71">
         <v>1744</v>
       </c>
       <c r="D264" s="4" t="s">
         <v>643</v>
       </c>
-      <c r="E264" s="76" t="s">
+      <c r="E264" s="72" t="s">
         <v>646</v>
       </c>
-      <c r="F264" s="78" t="s">
+      <c r="F264" s="74" t="s">
         <v>42</v>
       </c>
       <c r="G264" s="8"/>
@@ -9483,20 +9483,20 @@
       </c>
       <c r="I264" s="43"/>
     </row>
-    <row r="265" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B265" s="75">
+    <row r="265" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B265" s="71">
         <v>255</v>
       </c>
-      <c r="C265" s="75">
+      <c r="C265" s="71">
         <v>2772</v>
       </c>
       <c r="D265" s="4" t="s">
         <v>644</v>
       </c>
-      <c r="E265" s="76" t="s">
+      <c r="E265" s="72" t="s">
         <v>646</v>
       </c>
-      <c r="F265" s="78" t="s">
+      <c r="F265" s="74" t="s">
         <v>42</v>
       </c>
       <c r="G265" s="8"/>
@@ -9505,20 +9505,20 @@
       </c>
       <c r="I265" s="43"/>
     </row>
-    <row r="266" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B266" s="75">
+    <row r="266" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B266" s="71">
         <v>256</v>
       </c>
-      <c r="C266" s="79">
+      <c r="C266" s="82">
         <v>798</v>
       </c>
       <c r="D266" s="4" t="s">
         <v>645</v>
       </c>
-      <c r="E266" s="76" t="s">
+      <c r="E266" s="72" t="s">
         <v>646</v>
       </c>
-      <c r="F266" s="80" t="s">
+      <c r="F266" s="75" t="s">
         <v>60</v>
       </c>
       <c r="G266" s="8"/>
@@ -9527,797 +9527,797 @@
       </c>
       <c r="I266" s="43"/>
     </row>
-    <row r="267" spans="2:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B267" s="81" t="s">
+    <row r="267" spans="2:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B267" s="76" t="s">
         <v>546</v>
       </c>
-      <c r="C267" s="82"/>
-      <c r="D267" s="82"/>
-      <c r="E267" s="82"/>
-      <c r="F267" s="82"/>
-      <c r="G267" s="82"/>
-      <c r="H267" s="82"/>
-    </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C267" s="77"/>
+      <c r="D267" s="77"/>
+      <c r="E267" s="77"/>
+      <c r="F267" s="77"/>
+      <c r="G267" s="77"/>
+      <c r="H267" s="77"/>
+    </row>
+    <row r="295" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B295" s="19"/>
       <c r="F295" s="48"/>
       <c r="H295" s="49"/>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A296" s="70"/>
-      <c r="B296" s="72"/>
+    <row r="296" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A296" s="66"/>
+      <c r="B296" s="68"/>
       <c r="H296" s="49"/>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A297" s="70"/>
-      <c r="B297" s="69"/>
-      <c r="G297" s="69"/>
-      <c r="H297" s="69"/>
-    </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A298" s="70"/>
-      <c r="B298" s="74"/>
-      <c r="G298" s="70"/>
-      <c r="H298" s="71"/>
-    </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A299" s="70"/>
-      <c r="B299" s="73"/>
-      <c r="H299" s="66"/>
-    </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B300" s="65"/>
-      <c r="H300" s="66"/>
-    </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B301" s="64"/>
-      <c r="H301" s="66"/>
-    </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B302" s="64"/>
-      <c r="H302" s="66"/>
-    </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B303" s="65"/>
-      <c r="H303" s="66"/>
-    </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B304" s="65"/>
-      <c r="H304" s="66"/>
-    </row>
-    <row r="305" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B305" s="64"/>
-      <c r="H305" s="66"/>
-    </row>
-    <row r="306" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B306" s="64"/>
-      <c r="H306" s="66"/>
-    </row>
-    <row r="307" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B307" s="65"/>
-      <c r="H307" s="66"/>
-    </row>
-    <row r="308" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B308" s="65"/>
-      <c r="H308" s="66"/>
-    </row>
-    <row r="309" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B309" s="65"/>
-      <c r="H309" s="66"/>
-    </row>
-    <row r="310" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B310" s="65"/>
-      <c r="H310" s="66"/>
-    </row>
-    <row r="311" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B311" s="65"/>
-      <c r="H311" s="66"/>
-    </row>
-    <row r="312" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B312" s="64"/>
-      <c r="H312" s="66"/>
-    </row>
-    <row r="313" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B313" s="65"/>
-      <c r="H313" s="66"/>
-    </row>
-    <row r="314" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B314" s="65"/>
-      <c r="H314" s="66"/>
-    </row>
-    <row r="315" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B315" s="65"/>
-      <c r="H315" s="66"/>
-    </row>
-    <row r="316" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B316" s="65"/>
-      <c r="H316" s="66"/>
-    </row>
-    <row r="317" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B317" s="65"/>
-      <c r="H317" s="66"/>
-    </row>
-    <row r="318" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B318" s="65"/>
-      <c r="H318" s="66"/>
-    </row>
-    <row r="319" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B319" s="65"/>
-      <c r="H319" s="66"/>
-    </row>
-    <row r="320" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B320" s="65"/>
-      <c r="H320" s="66"/>
-    </row>
-    <row r="321" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B321" s="65"/>
-      <c r="H321" s="66"/>
-    </row>
-    <row r="322" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B322" s="65"/>
-      <c r="H322" s="66"/>
-    </row>
-    <row r="323" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B323" s="65"/>
-      <c r="H323" s="66"/>
-    </row>
-    <row r="324" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B324" s="65"/>
-      <c r="H324" s="66"/>
-    </row>
-    <row r="325" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B325" s="67"/>
-      <c r="H325" s="68"/>
-    </row>
-    <row r="326" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A297" s="66"/>
+      <c r="B297" s="65"/>
+      <c r="G297" s="65"/>
+      <c r="H297" s="65"/>
+    </row>
+    <row r="298" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A298" s="66"/>
+      <c r="B298" s="70"/>
+      <c r="G298" s="66"/>
+      <c r="H298" s="67"/>
+    </row>
+    <row r="299" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A299" s="66"/>
+      <c r="B299" s="69"/>
+      <c r="H299" s="62"/>
+    </row>
+    <row r="300" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B300" s="61"/>
+      <c r="H300" s="62"/>
+    </row>
+    <row r="301" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B301" s="60"/>
+      <c r="H301" s="62"/>
+    </row>
+    <row r="302" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B302" s="60"/>
+      <c r="H302" s="62"/>
+    </row>
+    <row r="303" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B303" s="61"/>
+      <c r="H303" s="62"/>
+    </row>
+    <row r="304" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B304" s="61"/>
+      <c r="H304" s="62"/>
+    </row>
+    <row r="305" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B305" s="60"/>
+      <c r="H305" s="62"/>
+    </row>
+    <row r="306" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B306" s="60"/>
+      <c r="H306" s="62"/>
+    </row>
+    <row r="307" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B307" s="61"/>
+      <c r="H307" s="62"/>
+    </row>
+    <row r="308" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B308" s="61"/>
+      <c r="H308" s="62"/>
+    </row>
+    <row r="309" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B309" s="61"/>
+      <c r="H309" s="62"/>
+    </row>
+    <row r="310" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B310" s="61"/>
+      <c r="H310" s="62"/>
+    </row>
+    <row r="311" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B311" s="61"/>
+      <c r="H311" s="62"/>
+    </row>
+    <row r="312" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B312" s="60"/>
+      <c r="H312" s="62"/>
+    </row>
+    <row r="313" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B313" s="61"/>
+      <c r="H313" s="62"/>
+    </row>
+    <row r="314" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B314" s="61"/>
+      <c r="H314" s="62"/>
+    </row>
+    <row r="315" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B315" s="61"/>
+      <c r="H315" s="62"/>
+    </row>
+    <row r="316" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B316" s="61"/>
+      <c r="H316" s="62"/>
+    </row>
+    <row r="317" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B317" s="61"/>
+      <c r="H317" s="62"/>
+    </row>
+    <row r="318" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B318" s="61"/>
+      <c r="H318" s="62"/>
+    </row>
+    <row r="319" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B319" s="61"/>
+      <c r="H319" s="62"/>
+    </row>
+    <row r="320" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B320" s="61"/>
+      <c r="H320" s="62"/>
+    </row>
+    <row r="321" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B321" s="61"/>
+      <c r="H321" s="62"/>
+    </row>
+    <row r="322" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B322" s="61"/>
+      <c r="H322" s="62"/>
+    </row>
+    <row r="323" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B323" s="61"/>
+      <c r="H323" s="62"/>
+    </row>
+    <row r="324" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B324" s="61"/>
+      <c r="H324" s="62"/>
+    </row>
+    <row r="325" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B325" s="63"/>
+      <c r="H325" s="64"/>
+    </row>
+    <row r="326" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C326" s="21"/>
       <c r="D326" s="22"/>
       <c r="E326" s="27"/>
       <c r="F326" s="28"/>
     </row>
-    <row r="327" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="327" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C327" s="21"/>
       <c r="D327" s="22"/>
       <c r="E327" s="27"/>
       <c r="F327" s="28"/>
     </row>
-    <row r="328" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="328" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C328" s="21"/>
       <c r="D328" s="22"/>
       <c r="E328" s="23"/>
       <c r="F328" s="28"/>
     </row>
-    <row r="329" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="329" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C329" s="21"/>
       <c r="D329" s="22"/>
       <c r="E329" s="23"/>
       <c r="F329" s="28"/>
     </row>
-    <row r="330" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="330" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C330" s="21"/>
       <c r="D330" s="22"/>
       <c r="E330" s="23"/>
       <c r="F330" s="28"/>
     </row>
-    <row r="331" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="331" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C331" s="21"/>
       <c r="D331" s="22"/>
       <c r="E331" s="27"/>
       <c r="F331" s="28"/>
     </row>
-    <row r="332" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="332" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C332" s="21"/>
       <c r="D332" s="22"/>
       <c r="E332" s="23"/>
       <c r="F332" s="28"/>
     </row>
-    <row r="333" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="333" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C333" s="21"/>
       <c r="D333" s="22"/>
       <c r="E333" s="27"/>
       <c r="F333" s="28"/>
     </row>
-    <row r="334" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="334" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C334" s="21"/>
       <c r="D334" s="22"/>
       <c r="E334" s="27"/>
       <c r="F334" s="28"/>
     </row>
-    <row r="335" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="335" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C335" s="21"/>
       <c r="D335" s="22"/>
       <c r="E335" s="23"/>
       <c r="F335" s="28"/>
     </row>
-    <row r="336" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="336" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C336" s="21"/>
       <c r="D336" s="22"/>
       <c r="E336" s="23"/>
       <c r="F336" s="28"/>
     </row>
-    <row r="337" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="337" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C337" s="21"/>
       <c r="D337" s="22"/>
       <c r="E337" s="23"/>
       <c r="F337" s="28"/>
     </row>
-    <row r="338" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="338" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C338" s="21"/>
       <c r="D338" s="22"/>
       <c r="E338" s="23"/>
       <c r="F338" s="28"/>
     </row>
-    <row r="339" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="339" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C339" s="21"/>
       <c r="D339" s="22"/>
       <c r="E339" s="23"/>
       <c r="F339" s="28"/>
     </row>
-    <row r="340" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="340" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C340" s="21"/>
       <c r="D340" s="22"/>
       <c r="E340" s="23"/>
       <c r="F340" s="28"/>
     </row>
-    <row r="341" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="341" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C341" s="21"/>
       <c r="D341" s="22"/>
       <c r="E341" s="23"/>
       <c r="F341" s="28"/>
     </row>
-    <row r="342" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="342" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C342" s="21"/>
       <c r="D342" s="22"/>
       <c r="E342" s="27"/>
       <c r="F342" s="28"/>
     </row>
-    <row r="343" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="343" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C343" s="21"/>
       <c r="D343" s="22"/>
       <c r="E343" s="27"/>
       <c r="F343" s="28"/>
     </row>
-    <row r="344" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="344" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C344" s="21"/>
       <c r="D344" s="22"/>
       <c r="E344" s="23"/>
       <c r="F344" s="28"/>
     </row>
-    <row r="345" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="345" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C345" s="21"/>
       <c r="D345" s="22"/>
       <c r="E345" s="23"/>
       <c r="F345" s="28"/>
     </row>
-    <row r="346" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="346" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C346" s="21"/>
       <c r="D346" s="22"/>
       <c r="E346" s="27"/>
       <c r="F346" s="28"/>
     </row>
-    <row r="347" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="347" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C347" s="21"/>
       <c r="D347" s="22"/>
       <c r="E347" s="23"/>
       <c r="F347" s="24"/>
     </row>
-    <row r="348" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="348" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C348" s="21"/>
       <c r="D348" s="22"/>
       <c r="E348" s="23"/>
       <c r="F348" s="24"/>
     </row>
-    <row r="349" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="349" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C349" s="21"/>
       <c r="D349" s="22"/>
       <c r="E349" s="23"/>
       <c r="F349" s="24"/>
     </row>
-    <row r="350" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="350" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C350" s="21"/>
       <c r="D350" s="22"/>
       <c r="E350" s="23"/>
       <c r="F350" s="24"/>
     </row>
-    <row r="351" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="351" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B351" s="29"/>
       <c r="C351" s="21"/>
       <c r="D351" s="22"/>
       <c r="E351" s="23"/>
       <c r="F351" s="24"/>
     </row>
-    <row r="352" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="352" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B352" s="19"/>
       <c r="C352" s="21"/>
       <c r="D352" s="22"/>
       <c r="E352" s="23"/>
       <c r="F352" s="24"/>
     </row>
-    <row r="353" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="353" spans="2:6" ht="17.75" x14ac:dyDescent="0.3">
       <c r="B353" s="20"/>
       <c r="C353" s="30"/>
       <c r="D353" s="30"/>
       <c r="E353" s="30"/>
       <c r="F353" s="30"/>
     </row>
-    <row r="354" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="354" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B354" s="20"/>
       <c r="C354" s="31"/>
       <c r="D354" s="32"/>
       <c r="E354" s="33"/>
       <c r="F354" s="34"/>
     </row>
-    <row r="355" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="355" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B355" s="19"/>
       <c r="C355" s="31"/>
       <c r="D355" s="32"/>
       <c r="E355" s="27"/>
       <c r="F355" s="35"/>
     </row>
-    <row r="356" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="356" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B356" s="19"/>
       <c r="C356" s="31"/>
       <c r="D356" s="32"/>
       <c r="E356" s="33"/>
       <c r="F356" s="35"/>
     </row>
-    <row r="357" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="357" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B357" s="20"/>
       <c r="C357" s="31"/>
       <c r="D357" s="32"/>
       <c r="E357" s="33"/>
       <c r="F357" s="35"/>
     </row>
-    <row r="358" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="358" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B358" s="19"/>
       <c r="C358" s="31"/>
       <c r="D358" s="32"/>
       <c r="E358" s="33"/>
       <c r="F358" s="35"/>
     </row>
-    <row r="359" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="359" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B359" s="19"/>
       <c r="C359" s="31"/>
       <c r="D359" s="32"/>
       <c r="E359" s="27"/>
       <c r="F359" s="35"/>
     </row>
-    <row r="360" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="360" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B360" s="19"/>
       <c r="C360" s="31"/>
       <c r="D360" s="32"/>
       <c r="E360" s="27"/>
       <c r="F360" s="36"/>
     </row>
-    <row r="361" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="361" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B361" s="19"/>
       <c r="C361" s="31"/>
       <c r="D361" s="32"/>
       <c r="E361" s="27"/>
       <c r="F361" s="36"/>
     </row>
-    <row r="362" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="362" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B362" s="19"/>
       <c r="C362" s="31"/>
       <c r="D362" s="32"/>
       <c r="E362" s="33"/>
       <c r="F362" s="36"/>
     </row>
-    <row r="363" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="363" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B363" s="19"/>
     </row>
-    <row r="364" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="364" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B364" s="19"/>
     </row>
-    <row r="365" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="365" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B365" s="19"/>
     </row>
-    <row r="366" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="366" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B366" s="19"/>
     </row>
-    <row r="367" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="367" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B367" s="19"/>
     </row>
-    <row r="368" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="368" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B368" s="19"/>
     </row>
-    <row r="369" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="369" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B369" s="20"/>
     </row>
-    <row r="370" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="370" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B370" s="19"/>
     </row>
-    <row r="371" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="371" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B371" s="19"/>
     </row>
-    <row r="372" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="372" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B372" s="19"/>
     </row>
-    <row r="373" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="373" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B373" s="19"/>
     </row>
-    <row r="374" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="374" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B374" s="19"/>
     </row>
-    <row r="375" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="375" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B375" s="19"/>
     </row>
-    <row r="376" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="376" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B376" s="20"/>
     </row>
-    <row r="377" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="377" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B377" s="19"/>
     </row>
-    <row r="378" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="378" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B378" s="19"/>
     </row>
-    <row r="379" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="379" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B379" s="20"/>
     </row>
-    <row r="380" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="380" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B380" s="19"/>
     </row>
-    <row r="381" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="381" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B381" s="19"/>
     </row>
-    <row r="382" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="382" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B382" s="19"/>
     </row>
-    <row r="383" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="383" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B383" s="19"/>
     </row>
-    <row r="384" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="384" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B384" s="19"/>
     </row>
-    <row r="385" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="385" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B385" s="19"/>
     </row>
-    <row r="386" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="386" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B386" s="19"/>
     </row>
-    <row r="387" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="387" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B387" s="19"/>
     </row>
-    <row r="388" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="388" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B388" s="19"/>
     </row>
-    <row r="389" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="389" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B389" s="19"/>
     </row>
-    <row r="390" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="390" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B390" s="19"/>
     </row>
-    <row r="391" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="391" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B391" s="19"/>
     </row>
-    <row r="392" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="392" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B392" s="19"/>
     </row>
-    <row r="393" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="393" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B393" s="19"/>
     </row>
-    <row r="394" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="394" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B394" s="19"/>
     </row>
-    <row r="395" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="395" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B395" s="20"/>
     </row>
-    <row r="396" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="396" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B396" s="19"/>
     </row>
-    <row r="397" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="397" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B397" s="19"/>
     </row>
-    <row r="398" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="398" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B398" s="19"/>
     </row>
-    <row r="399" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="399" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B399" s="19"/>
     </row>
-    <row r="400" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="400" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B400" s="19"/>
     </row>
-    <row r="401" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="401" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B401" s="19"/>
     </row>
-    <row r="402" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="402" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B402" s="19"/>
     </row>
-    <row r="403" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="403" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B403" s="19"/>
     </row>
-    <row r="404" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="404" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B404" s="19"/>
     </row>
-    <row r="405" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="405" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B405" s="19"/>
     </row>
-    <row r="406" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="406" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B406" s="19"/>
     </row>
-    <row r="407" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="407" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B407" s="19"/>
     </row>
-    <row r="408" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="408" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B408" s="19"/>
     </row>
-    <row r="409" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="409" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B409" s="19"/>
     </row>
-    <row r="410" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="410" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B410" s="19"/>
     </row>
-    <row r="411" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="411" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B411" s="19"/>
     </row>
-    <row r="412" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="412" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B412" s="19"/>
     </row>
-    <row r="413" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="413" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B413" s="19"/>
     </row>
-    <row r="414" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="414" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B414" s="19"/>
     </row>
-    <row r="415" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="415" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B415" s="20"/>
     </row>
-    <row r="416" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="416" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B416" s="19"/>
     </row>
-    <row r="417" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="417" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B417" s="19"/>
     </row>
-    <row r="418" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="418" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B418" s="19"/>
     </row>
-    <row r="419" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="419" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B419" s="19"/>
     </row>
-    <row r="420" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="420" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B420" s="19"/>
     </row>
-    <row r="421" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="421" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B421" s="19"/>
     </row>
-    <row r="422" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="422" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B422" s="19"/>
     </row>
-    <row r="423" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="423" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B423" s="19"/>
     </row>
-    <row r="424" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="424" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B424" s="19"/>
     </row>
-    <row r="425" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="425" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B425" s="19"/>
     </row>
-    <row r="426" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="426" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B426" s="19"/>
     </row>
-    <row r="427" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="427" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B427" s="19"/>
     </row>
-    <row r="428" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="428" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B428" s="19"/>
     </row>
-    <row r="429" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="429" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B429" s="19"/>
     </row>
-    <row r="430" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="430" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B430" s="19"/>
     </row>
-    <row r="431" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="431" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B431" s="19"/>
     </row>
-    <row r="432" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="432" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B432" s="19"/>
     </row>
-    <row r="433" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="433" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B433" s="20"/>
     </row>
-    <row r="434" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="434" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B434" s="19"/>
     </row>
-    <row r="435" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="435" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B435" s="19"/>
     </row>
-    <row r="436" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="436" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B436" s="19"/>
     </row>
-    <row r="437" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="437" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B437" s="19"/>
     </row>
-    <row r="438" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="438" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B438" s="19"/>
     </row>
-    <row r="439" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="439" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B439" s="19"/>
     </row>
-    <row r="440" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="440" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B440" s="19"/>
     </row>
-    <row r="441" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="441" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B441" s="19"/>
     </row>
-    <row r="442" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="442" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B442" s="20"/>
     </row>
-    <row r="443" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="443" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B443" s="19"/>
     </row>
-    <row r="444" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="444" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B444" s="19"/>
     </row>
-    <row r="445" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="445" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B445" s="19"/>
     </row>
-    <row r="446" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="446" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B446" s="19"/>
     </row>
-    <row r="447" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="447" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B447" s="19"/>
     </row>
-    <row r="448" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="448" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B448" s="19"/>
     </row>
-    <row r="449" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="449" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B449" s="19"/>
     </row>
-    <row r="450" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="450" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B450" s="19"/>
     </row>
-    <row r="451" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="451" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B451" s="19"/>
     </row>
-    <row r="452" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="452" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B452" s="19"/>
     </row>
-    <row r="453" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="453" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B453" s="19"/>
     </row>
-    <row r="454" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="454" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B454" s="19"/>
     </row>
-    <row r="455" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="455" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B455" s="19"/>
     </row>
-    <row r="456" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="456" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B456" s="19"/>
     </row>
-    <row r="457" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="457" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B457" s="19"/>
     </row>
-    <row r="458" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="458" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B458" s="19"/>
     </row>
-    <row r="459" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="459" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B459" s="19"/>
     </row>
-    <row r="460" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="460" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B460" s="19"/>
     </row>
-    <row r="461" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="461" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B461" s="19"/>
     </row>
-    <row r="462" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="462" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B462" s="19"/>
     </row>
-    <row r="463" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="463" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B463" s="19"/>
     </row>
-    <row r="464" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="464" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B464" s="19"/>
     </row>
-    <row r="465" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="465" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B465" s="19"/>
     </row>
-    <row r="466" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="466" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B466" s="19"/>
     </row>
-    <row r="467" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="467" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B467" s="19"/>
     </row>
-    <row r="468" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="468" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B468" s="19"/>
     </row>
-    <row r="469" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="469" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B469" s="19"/>
     </row>
-    <row r="470" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="470" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B470" s="20"/>
     </row>
-    <row r="471" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="471" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B471" s="19"/>
     </row>
-    <row r="472" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="472" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B472" s="19"/>
     </row>
-    <row r="473" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="473" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B473" s="19"/>
     </row>
-    <row r="474" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="474" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B474" s="19"/>
     </row>
-    <row r="475" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="475" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B475" s="19"/>
     </row>
-    <row r="476" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="476" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B476" s="19"/>
       <c r="C476" s="29"/>
       <c r="D476" s="29"/>
       <c r="E476" s="29"/>
       <c r="F476" s="39"/>
     </row>
-    <row r="477" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="477" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B477" s="40"/>
       <c r="C477" s="40"/>
       <c r="D477" s="40"/>
       <c r="E477" s="40"/>
       <c r="F477" s="27"/>
     </row>
-    <row r="478" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="478" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B478" s="29"/>
       <c r="C478" s="29"/>
       <c r="D478" s="29"/>
       <c r="E478" s="29"/>
       <c r="F478" s="39"/>
     </row>
-    <row r="479" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="479" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B479" s="19"/>
     </row>
-    <row r="480" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="480" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B480" s="20"/>
     </row>
-    <row r="481" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="481" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B481" s="20"/>
     </row>
-    <row r="482" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="482" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B482" s="41"/>
     </row>
-    <row r="483" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="483" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B483" s="19"/>
     </row>
-    <row r="484" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="484" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B484" s="19"/>
     </row>
-    <row r="485" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="485" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B485" s="19"/>
     </row>
-    <row r="486" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="486" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B486" s="19"/>
     </row>
-    <row r="487" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="487" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B487" s="19"/>
     </row>
-    <row r="488" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="488" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B488" s="20"/>
     </row>
-    <row r="489" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="489" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B489" s="19"/>
     </row>
-    <row r="490" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="490" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B490" s="19"/>
     </row>
-    <row r="491" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="491" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B491" s="19"/>
     </row>
-    <row r="492" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="492" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B492" s="19"/>
     </row>
-    <row r="493" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="493" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B493" s="20"/>
     </row>
-    <row r="494" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="494" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B494" s="20"/>
     </row>
-    <row r="495" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="495" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B495" s="19"/>
     </row>
-    <row r="496" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="496" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B496" s="19"/>
     </row>
-    <row r="497" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="497" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B497" s="19"/>
     </row>
   </sheetData>
@@ -10609,9 +10609,9 @@
       <selection sqref="A1:G56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="56" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="53.75" x14ac:dyDescent="0.3">
       <c r="A1" s="50">
         <v>229</v>
       </c>
@@ -10632,7 +10632,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="56" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="53.75" x14ac:dyDescent="0.3">
       <c r="A2" s="50">
         <v>230</v>
       </c>
@@ -10653,7 +10653,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="84" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="80.599999999999994" x14ac:dyDescent="0.3">
       <c r="A3" s="50">
         <v>231</v>
       </c>
@@ -10674,7 +10674,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="112" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="94.05" x14ac:dyDescent="0.3">
       <c r="A4" s="50">
         <v>232</v>
       </c>
@@ -10695,7 +10695,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="98" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="94.05" x14ac:dyDescent="0.3">
       <c r="A5" s="50">
         <v>233</v>
       </c>
@@ -10716,7 +10716,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="53.75" x14ac:dyDescent="0.3">
       <c r="A6" s="50">
         <v>234</v>
       </c>
@@ -10737,7 +10737,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="56" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="53.75" x14ac:dyDescent="0.3">
       <c r="A7" s="50">
         <v>235</v>
       </c>
@@ -10758,7 +10758,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A8" s="50">
         <v>236</v>
       </c>
@@ -10779,7 +10779,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="84" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="80.599999999999994" x14ac:dyDescent="0.3">
       <c r="A9" s="50">
         <v>237</v>
       </c>
@@ -10800,7 +10800,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="84" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="80.599999999999994" x14ac:dyDescent="0.3">
       <c r="A10" s="50">
         <v>238</v>
       </c>
@@ -10821,7 +10821,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="42" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="40.299999999999997" x14ac:dyDescent="0.3">
       <c r="A11" s="50">
         <v>239</v>
       </c>
@@ -10842,7 +10842,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="42" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="40.299999999999997" x14ac:dyDescent="0.3">
       <c r="A12" s="50">
         <v>240</v>
       </c>
@@ -10863,7 +10863,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A13" s="50">
         <v>241</v>
       </c>
@@ -10884,7 +10884,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A14" s="50">
         <v>242</v>
       </c>
@@ -10905,7 +10905,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="42" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="40.299999999999997" x14ac:dyDescent="0.3">
       <c r="A15" s="50">
         <v>243</v>
       </c>
@@ -10926,7 +10926,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="84" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="80.599999999999994" x14ac:dyDescent="0.3">
       <c r="A16" s="50">
         <v>244</v>
       </c>
@@ -10947,7 +10947,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="84" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="80.599999999999994" x14ac:dyDescent="0.3">
       <c r="A17" s="50">
         <v>245</v>
       </c>
@@ -10968,7 +10968,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A18" s="50">
         <v>246</v>
       </c>
@@ -10989,7 +10989,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A19" s="50">
         <v>247</v>
       </c>
@@ -11010,7 +11010,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="98" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="94.05" x14ac:dyDescent="0.3">
       <c r="A20" s="50">
         <v>248</v>
       </c>
@@ -11031,7 +11031,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A21" s="50">
         <v>249</v>
       </c>
@@ -11052,7 +11052,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="84" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="80.599999999999994" x14ac:dyDescent="0.3">
       <c r="A22" s="50">
         <v>250</v>
       </c>
@@ -11073,7 +11073,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A23" s="50">
         <v>251</v>
       </c>
@@ -11094,7 +11094,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="140" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="134.35" x14ac:dyDescent="0.3">
       <c r="A24" s="50">
         <v>252</v>
       </c>
@@ -11115,7 +11115,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="98" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="94.05" x14ac:dyDescent="0.3">
       <c r="A25" s="50">
         <v>253</v>
       </c>
@@ -11136,7 +11136,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="84" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="80.599999999999994" x14ac:dyDescent="0.3">
       <c r="A26" s="50">
         <v>254</v>
       </c>
@@ -11157,7 +11157,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A27" s="50">
         <v>255</v>
       </c>
@@ -11178,7 +11178,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="126" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="120.9" x14ac:dyDescent="0.3">
       <c r="A28" s="50">
         <v>256</v>
       </c>
@@ -11199,7 +11199,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A29" s="50">
         <v>257</v>
       </c>
@@ -11220,7 +11220,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="80.599999999999994" x14ac:dyDescent="0.3">
       <c r="A30" s="50">
         <v>258</v>
       </c>
@@ -11241,7 +11241,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="98" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="94.05" x14ac:dyDescent="0.3">
       <c r="A31" s="50">
         <v>259</v>
       </c>
@@ -11262,7 +11262,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A32" s="50">
         <v>260</v>
       </c>
@@ -11283,7 +11283,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A33" s="50">
         <v>261</v>
       </c>
@@ -11304,7 +11304,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A34" s="50">
         <v>262</v>
       </c>
@@ -11325,7 +11325,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A35" s="50">
         <v>263</v>
       </c>
@@ -11346,7 +11346,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="84" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="80.599999999999994" x14ac:dyDescent="0.3">
       <c r="A36" s="50">
         <v>264</v>
       </c>
@@ -11367,7 +11367,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A37" s="50">
         <v>265</v>
       </c>
@@ -11388,7 +11388,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A38" s="50">
         <v>266</v>
       </c>
@@ -11409,7 +11409,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A39" s="50">
         <v>267</v>
       </c>
@@ -11430,7 +11430,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A40" s="50">
         <v>268</v>
       </c>
@@ -11451,7 +11451,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A41" s="50">
         <v>269</v>
       </c>
@@ -11472,7 +11472,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A42" s="50">
         <v>270</v>
       </c>
@@ -11493,7 +11493,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A43" s="50">
         <v>271</v>
       </c>
@@ -11514,7 +11514,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="98" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="94.05" x14ac:dyDescent="0.3">
       <c r="A44" s="50">
         <v>272</v>
       </c>
@@ -11535,7 +11535,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A45" s="50">
         <v>273</v>
       </c>
@@ -11556,7 +11556,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="84" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" ht="80.599999999999994" x14ac:dyDescent="0.3">
       <c r="A46" s="50">
         <v>274</v>
       </c>
@@ -11577,7 +11577,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A47" s="50">
         <v>275</v>
       </c>
@@ -11598,7 +11598,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="84" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" ht="80.599999999999994" x14ac:dyDescent="0.3">
       <c r="A48" s="50">
         <v>276</v>
       </c>
@@ -11619,7 +11619,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A49" s="50">
         <v>277</v>
       </c>
@@ -11640,7 +11640,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A50" s="50">
         <v>278</v>
       </c>
@@ -11661,7 +11661,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="98" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" ht="94.05" x14ac:dyDescent="0.3">
       <c r="A51" s="50">
         <v>279</v>
       </c>
@@ -11682,7 +11682,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A52" s="50">
         <v>280</v>
       </c>
@@ -11703,7 +11703,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="84" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" ht="80.599999999999994" x14ac:dyDescent="0.3">
       <c r="A53" s="50">
         <v>281</v>
       </c>
@@ -11724,7 +11724,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A54" s="50">
         <v>282</v>
       </c>
@@ -11745,7 +11745,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A55" s="50">
         <v>283</v>
       </c>
@@ -11766,7 +11766,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A56" s="50">
         <v>284</v>
       </c>

</xml_diff>